<commit_message>
Update Dockerfile, README and SQLITE3 connection
</commit_message>
<xml_diff>
--- a/index_output.xlsx
+++ b/index_output.xlsx
@@ -551,13 +551,13 @@
         <v>45820</v>
       </c>
       <c r="B8" t="n">
-        <v>100.9454</v>
+        <v>100.7893</v>
       </c>
       <c r="C8" t="n">
-        <v>0.003264</v>
+        <v>0.001712</v>
       </c>
       <c r="D8" t="n">
-        <v>0.009454000000000073</v>
+        <v>0.007892999999999928</v>
       </c>
     </row>
     <row r="9">
@@ -565,13 +565,13 @@
         <v>45821</v>
       </c>
       <c r="B9" t="n">
-        <v>99.4706</v>
+        <v>99.3168</v>
       </c>
       <c r="C9" t="n">
         <v>-0.014609</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.00529399999999991</v>
+        <v>-0.006831999999999949</v>
       </c>
     </row>
     <row r="10">
@@ -579,13 +579,13 @@
         <v>45824</v>
       </c>
       <c r="B10" t="n">
-        <v>100.4257</v>
+        <v>100.2704</v>
       </c>
       <c r="C10" t="n">
         <v>0.009601</v>
       </c>
       <c r="D10" t="n">
-        <v>0.004256999999999955</v>
+        <v>0.00270400000000004</v>
       </c>
     </row>
     <row r="11">
@@ -593,13 +593,13 @@
         <v>45825</v>
       </c>
       <c r="B11" t="n">
-        <v>99.5321</v>
+        <v>99.37820000000001</v>
       </c>
       <c r="C11" t="n">
         <v>-0.008898</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.004678999999999989</v>
+        <v>-0.006217999999999946</v>
       </c>
     </row>
     <row r="12">
@@ -607,13 +607,13 @@
         <v>45826</v>
       </c>
       <c r="B12" t="n">
-        <v>99.1641</v>
+        <v>99.0108</v>
       </c>
       <c r="C12" t="n">
         <v>-0.003697</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.008359000000000005</v>
+        <v>-0.009892000000000012</v>
       </c>
     </row>
     <row r="13">
@@ -621,13 +621,13 @@
         <v>45828</v>
       </c>
       <c r="B13" t="n">
-        <v>98.89360000000001</v>
+        <v>98.7406</v>
       </c>
       <c r="C13" t="n">
         <v>-0.002729</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.01106399999999996</v>
+        <v>-0.01259399999999999</v>
       </c>
     </row>
     <row r="14">
@@ -635,13 +635,13 @@
         <v>45831</v>
       </c>
       <c r="B14" t="n">
-        <v>100.6073</v>
+        <v>100.4518</v>
       </c>
       <c r="C14" t="n">
         <v>0.017329</v>
       </c>
       <c r="D14" t="n">
-        <v>0.006072999999999995</v>
+        <v>0.004518000000000022</v>
       </c>
     </row>
     <row r="15">
@@ -649,13 +649,13 @@
         <v>45832</v>
       </c>
       <c r="B15" t="n">
-        <v>102.1243</v>
+        <v>101.9682</v>
       </c>
       <c r="C15" t="n">
-        <v>0.015078</v>
+        <v>0.015096</v>
       </c>
       <c r="D15" t="n">
-        <v>0.02124300000000012</v>
+        <v>0.01968199999999998</v>
       </c>
     </row>
     <row r="16">
@@ -663,13 +663,13 @@
         <v>45833</v>
       </c>
       <c r="B16" t="n">
-        <v>102.0145</v>
+        <v>101.8586</v>
       </c>
       <c r="C16" t="n">
         <v>-0.001075</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02014500000000008</v>
+        <v>0.01858599999999999</v>
       </c>
     </row>
     <row r="17">
@@ -677,13 +677,13 @@
         <v>45834</v>
       </c>
       <c r="B17" t="n">
-        <v>103.064</v>
+        <v>102.9065</v>
       </c>
       <c r="C17" t="n">
         <v>0.010288</v>
       </c>
       <c r="D17" t="n">
-        <v>0.03064</v>
+        <v>0.0290649999999999</v>
       </c>
     </row>
     <row r="18">
@@ -691,13 +691,13 @@
         <v>45835</v>
       </c>
       <c r="B18" t="n">
-        <v>103.707</v>
+        <v>103.5485</v>
       </c>
       <c r="C18" t="n">
         <v>0.006239</v>
       </c>
       <c r="D18" t="n">
-        <v>0.03706999999999994</v>
+        <v>0.03548499999999999</v>
       </c>
     </row>
     <row r="19">
@@ -705,13 +705,13 @@
         <v>45838</v>
       </c>
       <c r="B19" t="n">
-        <v>104.6447</v>
+        <v>104.4848</v>
       </c>
       <c r="C19" t="n">
         <v>0.009042</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04644699999999991</v>
+        <v>0.044848</v>
       </c>
     </row>
     <row r="20">
@@ -719,13 +719,13 @@
         <v>45839</v>
       </c>
       <c r="B20" t="n">
-        <v>104.309</v>
+        <v>104.1496</v>
       </c>
       <c r="C20" t="n">
         <v>-0.003208</v>
       </c>
       <c r="D20" t="n">
-        <v>0.04309000000000007</v>
+        <v>0.04149599999999998</v>
       </c>
     </row>
     <row r="21">
@@ -733,13 +733,13 @@
         <v>45840</v>
       </c>
       <c r="B21" t="n">
-        <v>104.4013</v>
+        <v>104.2418</v>
       </c>
       <c r="C21" t="n">
         <v>0.000885</v>
       </c>
       <c r="D21" t="n">
-        <v>0.04401300000000008</v>
+        <v>0.04241800000000007</v>
       </c>
     </row>
     <row r="22">
@@ -747,13 +747,13 @@
         <v>45841</v>
       </c>
       <c r="B22" t="n">
-        <v>105.235</v>
+        <v>105.0741</v>
       </c>
       <c r="C22" t="n">
         <v>0.007985000000000001</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0523499999999999</v>
+        <v>0.05074099999999993</v>
       </c>
     </row>
   </sheetData>
@@ -793,7 +793,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,GE,IBM,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,PGR,SPGI,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,ICE,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,GE,IBM,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,PGR,SPGI,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,ICE,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,GE,IBM,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,PGR,SPGI,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,ICE,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -823,7 +823,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,GE,IBM,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,PGR,SPGI,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -833,7 +833,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,GE,IBM,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,PGR,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -843,7 +843,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,GE,IBM,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,PGR,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,BMY,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,PGR,SPGI,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -863,7 +863,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,PGR,SPGI,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,ICE,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,PGR,SPGI,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,ICE,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,PGR,SPGI,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,ICE,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,PGR,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,ICE,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,PGR,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,ICE,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,AMT,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,PGR,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,AMT,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -923,7 +923,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,AMT,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,PGR,BSX,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,AMT,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,BSX,PGR,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,ICE,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -943,7 +943,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,DHR,ETN,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,BSX,PGR,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -953,7 +953,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,ETN,DHR,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,GE,IBM,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,BSX,PGR,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -963,7 +963,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,ETN,DHR,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,GE,IBM,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,ICE,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,ETN,DE,BA,CRM,LIN,AXP,SPGI,BSX,PGR,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,ICE,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,ETN,DHR,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,ETN,DE,BA,CRM,LIN,AXP,SPGI,BSX,PGR,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,ETN,DHR,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,DE,ETN,BA,CRM,LIN,AXP,SPGI,BSX,PGR,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>NVDA,TSLA,GOOGL,AMD,MRK,PEP,KKR,TMO,RTX,KLAC,AMGN,UNH,HD,ETN,DHR,ABBV,PM,AMAT,ADI,GS,AXP,MA,ISRG,BAC,MDT,TMUS,LMT,XOM,ORCL,SCHW,NFLX,BKNG,TJX,SBUX,GILD,INTU,JNJ,CVX,PG,COF,UBER,MSFT,AAPL,IBM,GE,KO,T,COP,NEE,CRWD,PANW,LOW,MCD,LLY,BX,DIS,CAT,PGR,LIN,VRTX,BLK,AVGO,GEV,LRCX,TXN,QCOM,CRM,JPM,HON,SPGI,CSCO,CMCSA,COST,ADP,GOOG,C,AMZN,WMT,MU,BA,CB,PFE,NOW,ABT,ANET,APH,V,ADBE,DE,META,BRK-B,MMC,MS,UNP,ACN,VZ,PLTR,WFC,BSX,SYK</t>
+          <t>AMZN,JNJ,GOOG,ABBV,AMD,C,GOOGL,COP,HD,GEV,XOM,CB,NVDA,AAPL,LRCX,GS,SYK,TJX,PLTR,KKR,PEP,COST,CRWD,ETN,DE,BA,CRM,LIN,AXP,SPGI,BSX,PGR,ORCL,MS,TSLA,ADBE,ISRG,VZ,TMO,BRK-B,LOW,CMCSA,WMT,ADI,UBER,DIS,ABT,ADP,BAC,SBUX,DHR,APH,AMGN,WFC,PG,SCHW,INTU,PM,AVGO,NEE,ANET,NFLX,MDT,NOW,QCOM,UNH,UNP,RTX,JPM,MU,AMAT,HON,V,MA,BKNG,GE,IBM,GILD,VRTX,BX,T,PANW,KO,KLAC,MCD,BLK,MMC,ACN,LMT,TXN,CAT,PFE,TMUS,CVX,COF,CSCO,MRK,MSFT,META,LLY</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LOW,MCD,LLY,NVDA,TSLA,GOOGL,BX,DIS,AMD,MRK,PEP,CAT,PGR,LIN,VRTX,BLK,AVGO,KKR,GEV,LRCX,TXN,TMO,QCOM,RTX,CRM,KLAC,AMGN,UNH,JPM,HON,SPGI,HD,DHR,ETN,CSCO,ABBV,PM,CMCSA,COST,AMAT,ADI,ADP,GOOG,GS,ICE,AXP,C,MA,ISRG,BAC,MDT,AMZN,WMT,TMUS,MU,BA,LMT,CB,PFE,XOM,ORCL,SCHW,NFLX,NOW,ABT,BKNG,TJX,ANET,APH,GILD,V,ADBE,INTU,DE,JNJ,CVX,PG,COF,META,UBER,MSFT,BRK-B,AAPL,GE,IBM,MMC,KO,MS,UNP,ACN,VZ,PLTR,T,WFC,COP,BSX,NEE,SYK,CRWD,PANW</t>
+          <t>ADP,AMZN,BAC,JNJ,DHR,GOOG,APH,ABBV,AMD,C,AMGN,WFC,GOOGL,COP,HD,GEV,PG,SCHW,INTU,PM,XOM,CB,AVGO,NEE,ANET,NVDA,AAPL,NFLX,LRCX,GS,MDT,NOW,QCOM,UNH,UNP,SYK,TJX,RTX,JPM,MU,AMAT,PLTR,HON,V,MA,KKR,PEP,BKNG,COST,GE,IBM,GILD,CRWD,VRTX,ICE,BX,T,PANW,KO,KLAC,MCD,DE,ETN,BA,BLK,MMC,ACN,LMT,CRM,LIN,TXN,AXP,CAT,PFE,PGR,SPGI,BSX,ORCL,MS,TMUS,CVX,TSLA,ADBE,COF,ISRG,VZ,CSCO,TMO,BRK-B,LOW,MRK,CMCSA,WMT,ADI,MSFT,META,LLY,UBER,DIS,ABT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -1091,16 +1091,8 @@
       <c r="A8" s="2" t="n">
         <v>45820</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>BMY</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>BX</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1113,7 +1105,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BMY</t>
+          <t>BX</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1301,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>45831</v>
@@ -1324,7 +1316,7 @@
         <v>-0.014609</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0523499999999999</v>
+        <v>0.05074099999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>